<commit_message>
Suppression des champs adresses MO dans la nomenclature opendata
</commit_message>
<xml_diff>
--- a/scripts/opendata/nomenclature_shapefile_des_reseaux_de_chaleur_et_froid.xlsx
+++ b/scripts/opendata/nomenclature_shapefile_des_reseaux_de_chaleur_et_froid.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\florence.levy\Downloads\opendata_fcu_101224\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\florence.levy\Downloads\opendata-fcu-150525\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A72300D-3119-49F0-834B-028D9529AC91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8899A4-98A1-45ED-AA76-6B71F479A207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="réseaux de chaleur - Nomenclatu" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="189">
   <si>
     <t>Nomenclature shapefile des réseaux de chaleur</t>
   </si>
@@ -72,24 +72,6 @@
   </si>
   <si>
     <t>MO</t>
-  </si>
-  <si>
-    <t>Adresse du MO</t>
-  </si>
-  <si>
-    <t>adresse_mo</t>
-  </si>
-  <si>
-    <t>Code postal du MO</t>
-  </si>
-  <si>
-    <t>CP_MO</t>
-  </si>
-  <si>
-    <t>Ville du MO</t>
-  </si>
-  <si>
-    <t>ville_mo</t>
   </si>
   <si>
     <t>Réseaux classés (checked=oui)</t>
@@ -2111,10 +2093,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -2233,13 +2215,13 @@
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
@@ -2247,13 +2229,13 @@
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>20</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
@@ -2261,13 +2243,13 @@
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
@@ -2275,13 +2257,13 @@
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
@@ -2289,13 +2271,13 @@
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
@@ -2303,13 +2285,13 @@
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
@@ -2317,13 +2299,13 @@
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
@@ -2331,13 +2313,13 @@
     </row>
     <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="7"/>
@@ -2345,13 +2327,13 @@
     </row>
     <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
@@ -2359,13 +2341,13 @@
     </row>
     <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="7"/>
@@ -2373,10 +2355,10 @@
     </row>
     <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>43</v>
@@ -2435,7 +2417,7 @@
         <v>51</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="7"/>
@@ -2443,13 +2425,13 @@
     </row>
     <row r="24" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
@@ -2457,13 +2439,13 @@
     </row>
     <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="7"/>
@@ -2471,13 +2453,13 @@
     </row>
     <row r="26" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="12" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="7"/>
@@ -2485,13 +2467,13 @@
     </row>
     <row r="27" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="7"/>
@@ -2499,13 +2481,13 @@
     </row>
     <row r="28" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="7"/>
@@ -2513,13 +2495,13 @@
     </row>
     <row r="29" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="12" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="7"/>
@@ -2527,13 +2509,13 @@
     </row>
     <row r="30" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="12" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="7"/>
@@ -2541,13 +2523,13 @@
     </row>
     <row r="31" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="12" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
@@ -2555,13 +2537,13 @@
     </row>
     <row r="32" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="12" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="7"/>
@@ -2569,13 +2551,13 @@
     </row>
     <row r="33" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="7"/>
@@ -2583,13 +2565,13 @@
     </row>
     <row r="34" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="12" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="7"/>
@@ -2597,13 +2579,13 @@
     </row>
     <row r="35" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="12" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="7"/>
@@ -2611,13 +2593,13 @@
     </row>
     <row r="36" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="12" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="7"/>
@@ -2625,13 +2607,13 @@
     </row>
     <row r="37" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="12" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="7"/>
@@ -2639,13 +2621,13 @@
     </row>
     <row r="38" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="12" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="7"/>
@@ -2653,13 +2635,13 @@
     </row>
     <row r="39" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="12" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="7"/>
@@ -2667,13 +2649,13 @@
     </row>
     <row r="40" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="12" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="7"/>
@@ -2681,55 +2663,55 @@
     </row>
     <row r="41" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="12" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="7"/>
       <c r="F41" s="8"/>
     </row>
-    <row r="42" spans="1:6" ht="20.100000000000001" customHeight="1">
+    <row r="42" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="12" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>105</v>
+        <v>170</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="7"/>
       <c r="F42" s="8"/>
     </row>
-    <row r="43" spans="1:6" ht="20.100000000000001" customHeight="1">
+    <row r="43" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="12" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>108</v>
+        <v>171</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>109</v>
+        <v>164</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="7"/>
       <c r="F43" s="8"/>
     </row>
-    <row r="44" spans="1:6" ht="20.100000000000001" customHeight="1">
+    <row r="44" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="12" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>111</v>
+        <v>172</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>112</v>
+        <v>165</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="7"/>
@@ -2737,13 +2719,13 @@
     </row>
     <row r="45" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="12" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="7"/>
@@ -2751,13 +2733,13 @@
     </row>
     <row r="46" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="7"/>
@@ -2765,13 +2747,13 @@
     </row>
     <row r="47" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="12" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="7"/>
@@ -2779,13 +2761,13 @@
     </row>
     <row r="48" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="12" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="7"/>
@@ -2793,13 +2775,13 @@
     </row>
     <row r="49" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="12" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="7"/>
@@ -2807,13 +2789,13 @@
     </row>
     <row r="50" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="7"/>
@@ -2821,13 +2803,13 @@
     </row>
     <row r="51" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="7"/>
@@ -2835,13 +2817,13 @@
     </row>
     <row r="52" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="7"/>
@@ -2849,13 +2831,13 @@
     </row>
     <row r="53" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="12" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="7"/>
@@ -2863,13 +2845,13 @@
     </row>
     <row r="54" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A54" s="12" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="7"/>
@@ -2877,13 +2859,13 @@
     </row>
     <row r="55" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="7"/>
@@ -2891,13 +2873,13 @@
     </row>
     <row r="56" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A56" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="7"/>
@@ -2905,13 +2887,13 @@
     </row>
     <row r="57" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A57" s="12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="7"/>
@@ -2919,13 +2901,13 @@
     </row>
     <row r="58" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="7"/>
@@ -2933,55 +2915,55 @@
     </row>
     <row r="59" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A59" s="12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="7"/>
       <c r="F59" s="8"/>
     </row>
-    <row r="60" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="60" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A60" s="12" t="s">
-        <v>155</v>
+        <v>107</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>191</v>
+        <v>108</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>161</v>
+        <v>109</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="7"/>
       <c r="F60" s="8"/>
     </row>
-    <row r="61" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="61" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A61" s="12" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>192</v>
+        <v>111</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="7"/>
       <c r="F61" s="8"/>
     </row>
-    <row r="62" spans="1:6" s="18" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="62" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A62" s="12" t="s">
-        <v>157</v>
+        <v>113</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>193</v>
+        <v>114</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>159</v>
+        <v>115</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="7"/>
@@ -2989,13 +2971,13 @@
     </row>
     <row r="63" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A63" s="12" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="7"/>
@@ -3003,13 +2985,13 @@
     </row>
     <row r="64" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A64" s="12" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="7"/>
@@ -3017,13 +2999,13 @@
     </row>
     <row r="65" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A65" s="12" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D65" s="6"/>
       <c r="E65" s="7"/>
@@ -3031,13 +3013,13 @@
     </row>
     <row r="66" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A66" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D66" s="6"/>
       <c r="E66" s="7"/>
@@ -3045,13 +3027,13 @@
     </row>
     <row r="67" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A67" s="12" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D67" s="6"/>
       <c r="E67" s="7"/>
@@ -3059,59 +3041,17 @@
     </row>
     <row r="68" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A68" s="12" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="D68" s="6"/>
-      <c r="E68" s="7"/>
-      <c r="F68" s="8"/>
-    </row>
-    <row r="69" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A69" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B69" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C69" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D69" s="6"/>
-      <c r="E69" s="7"/>
-      <c r="F69" s="8"/>
-    </row>
-    <row r="70" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A70" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B70" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C70" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D70" s="6"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="8"/>
-    </row>
-    <row r="71" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A71" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="B71" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="C71" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="D71" s="15"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="17"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3130,10 +3070,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -3147,7 +3087,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="27.6" customHeight="1">
       <c r="A1" s="20" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="19"/>
@@ -3161,7 +3101,7 @@
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="7"/>
@@ -3253,13 +3193,13 @@
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
@@ -3267,13 +3207,13 @@
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="12" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
@@ -3281,13 +3221,13 @@
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="12" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
@@ -3295,13 +3235,13 @@
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
@@ -3309,13 +3249,13 @@
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="12" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
@@ -3323,13 +3263,13 @@
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
@@ -3337,13 +3277,13 @@
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="12" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
@@ -3351,13 +3291,13 @@
     </row>
     <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="12" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="7"/>
@@ -3365,13 +3305,13 @@
     </row>
     <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="12" t="s">
-        <v>41</v>
+        <v>134</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>42</v>
+        <v>170</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>43</v>
+        <v>188</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
@@ -3379,13 +3319,13 @@
     </row>
     <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="12" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="7"/>
@@ -3393,13 +3333,13 @@
     </row>
     <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="12" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>61</v>
+        <v>112</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="7"/>
@@ -3407,13 +3347,13 @@
     </row>
     <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="12" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>176</v>
+        <v>114</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>194</v>
+        <v>115</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="7"/>
@@ -3421,13 +3361,13 @@
     </row>
     <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="12" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
@@ -3435,13 +3375,13 @@
     </row>
     <row r="22" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="12" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="7"/>
@@ -3449,59 +3389,17 @@
     </row>
     <row r="23" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="12" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C24" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A26" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="17"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>